<commit_message>
Added input to array
</commit_message>
<xml_diff>
--- a/data/model_data/testing2.xlsx
+++ b/data/model_data/testing2.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E4"/>
+  <dimension ref="A1:E1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -448,63 +448,6 @@
         </is>
       </c>
     </row>
-    <row r="2">
-      <c r="A2" t="n">
-        <v>1</v>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>Eldevin</t>
-        </is>
-      </c>
-      <c r="C2" t="n">
-        <v>1</v>
-      </c>
-      <c r="D2" t="n">
-        <v>1</v>
-      </c>
-      <c r="E2" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="n">
-        <v>1</v>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>BioShock</t>
-        </is>
-      </c>
-      <c r="C3" t="n">
-        <v>1</v>
-      </c>
-      <c r="D3" t="n">
-        <v>1</v>
-      </c>
-      <c r="E3" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="n">
-        <v>1</v>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>Jazzpunk</t>
-        </is>
-      </c>
-      <c r="C4" t="n">
-        <v>1</v>
-      </c>
-      <c r="D4" t="n">
-        <v>1</v>
-      </c>
-      <c r="E4" t="n">
-        <v>1</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>